<commit_message>
split CI; added bayesian regression
</commit_message>
<xml_diff>
--- a/drug_name_rework.xlsx
+++ b/drug_name_rework.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Documents\HNSCC_functional_data_pipeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8FF134-8904-4729-A020-C1E13D67BFC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F289CA4-F0F7-4974-92B6-5DD536A6A886}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{02ACD65C-6B84-4C18-8D72-904F0AF0430A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="438">
   <si>
     <t>Sunitinib;Malate;Romidepsin</t>
   </si>
@@ -1183,9 +1183,6 @@
   </si>
   <si>
     <t>correct_name_CAPS</t>
-  </si>
-  <si>
-    <t>primary_target</t>
   </si>
   <si>
     <t>target_ref</t>
@@ -1740,7 +1737,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
+      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1776,11 +1773,8 @@
       <c r="G1" t="s">
         <v>253</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>384</v>
-      </c>
-      <c r="I1" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -1812,14 +1806,14 @@
         <v>111</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>PELITINIB</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -1851,14 +1845,14 @@
         <v>114</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>MIDOSTAURIN</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -1885,7 +1879,7 @@
         <v>CERITINIB</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -1893,14 +1887,14 @@
         <v>117</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>TAMATINIB</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -1944,14 +1938,14 @@
         <v>121</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C14" s="1" t="str">
         <f t="shared" si="0"/>
         <v>LUTEOLIN</v>
       </c>
       <c r="G14" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -2013,7 +2007,7 @@
         <v>126</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C19" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2097,17 +2091,17 @@
         <v>133</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C26" s="1" t="str">
         <f t="shared" si="0"/>
         <v>AFATINIB DIMALEATE</v>
       </c>
       <c r="F26" t="s">
+        <v>401</v>
+      </c>
+      <c r="G26" t="s">
         <v>402</v>
-      </c>
-      <c r="G26" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
@@ -2422,7 +2416,7 @@
         <v>158</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C51" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2440,14 +2434,14 @@
         <v>159</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C52" s="2" t="str">
         <f t="shared" si="0"/>
         <v>SUNITINIB MALATE</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G52" s="3" t="s">
         <v>269</v>
@@ -2602,7 +2596,7 @@
         <v>172</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C65" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2911,17 +2905,17 @@
         <v>195</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C88" s="2" t="str">
         <f t="shared" si="1"/>
         <v>LAPATINIB DITOSYLATE</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.35">
@@ -3082,7 +3076,7 @@
         <v>208</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C101" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3229,7 +3223,7 @@
         <v>219</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C112" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3274,7 +3268,7 @@
         <v>222</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C115" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3367,7 +3361,7 @@
         <v>229</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C122" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3614,7 +3608,7 @@
         <v>3</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C139" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3674,7 +3668,7 @@
         <v>25</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C142" s="1" t="str">
         <f t="shared" si="2"/>
@@ -5320,7 +5314,7 @@
         <v>73</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C224" s="2" t="str">
         <f t="shared" si="5"/>
@@ -5740,10 +5734,10 @@
     </row>
     <row r="245" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A245" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B245" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C245" s="6" t="str">
         <f t="shared" si="5"/>
@@ -5752,10 +5746,10 @@
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A246" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C246" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5764,10 +5758,10 @@
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A247" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C247" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5776,10 +5770,10 @@
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A248" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C248" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5796,10 +5790,10 @@
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A249" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C249" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5816,10 +5810,10 @@
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A250" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C250" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5836,10 +5830,10 @@
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A251" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C251" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5856,10 +5850,10 @@
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A252" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C252" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5876,10 +5870,10 @@
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A253" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C253" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5896,10 +5890,10 @@
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A254" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C254" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5916,10 +5910,10 @@
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A255" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C255" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5936,10 +5930,10 @@
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A256" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C256" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5956,10 +5950,10 @@
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A257" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C257" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5976,10 +5970,10 @@
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A258" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C258" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5996,10 +5990,10 @@
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A259" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C259" s="1" t="str">
         <f t="shared" ref="C259:C270" si="10">UPPER(B259)</f>
@@ -6016,10 +6010,10 @@
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A260" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C260" s="1" t="str">
         <f t="shared" si="10"/>
@@ -6036,10 +6030,10 @@
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A261" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C261" s="1" t="str">
         <f t="shared" si="10"/>
@@ -6056,10 +6050,10 @@
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A262" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C262" s="1" t="str">
         <f t="shared" si="10"/>
@@ -6076,10 +6070,10 @@
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A263" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C263" s="1" t="str">
         <f t="shared" si="10"/>
@@ -6096,10 +6090,10 @@
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A264" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C264" s="1" t="str">
         <f t="shared" si="10"/>
@@ -6116,10 +6110,10 @@
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A265" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C265" s="1" t="str">
         <f t="shared" si="10"/>
@@ -6136,10 +6130,10 @@
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A266" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C266" s="1" t="str">
         <f t="shared" si="10"/>
@@ -6156,10 +6150,10 @@
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A267" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C267" s="1" t="str">
         <f t="shared" si="10"/>
@@ -6176,10 +6170,10 @@
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A268" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C268" s="1" t="str">
         <f t="shared" si="10"/>
@@ -6196,10 +6190,10 @@
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A269" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C269" s="1" t="str">
         <f t="shared" si="10"/>
@@ -6216,10 +6210,10 @@
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A270" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C270" s="1" t="str">
         <f t="shared" si="10"/>

</xml_diff>